<commit_message>
TryOptimization.py not sure if it will work
</commit_message>
<xml_diff>
--- a/data/generator/WindSolarConstraint.xlsx
+++ b/data/generator/WindSolarConstraint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meiyewang/Desktop/code/data/generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4D19C5-F0CF-F742-98D5-E45D4CA9599C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14258E23-059C-254F-B0E1-DFF344119967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15620" xr2:uid="{CED7BF43-EBD4-5348-B46C-0A9C3E97CC73}"/>
+    <workbookView xWindow="6540" yWindow="4520" windowWidth="27640" windowHeight="15620" xr2:uid="{CED7BF43-EBD4-5348-B46C-0A9C3E97CC73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,8 +485,8 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1">
-        <v>2.5673630999999999E-2</v>
+      <c r="B3">
+        <v>2.5673629999999999E-2</v>
       </c>
       <c r="C3">
         <v>0</v>

</xml_diff>